<commit_message>
clean files and codes
</commit_message>
<xml_diff>
--- a/analysis_result.xlsx
+++ b/analysis_result.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="trained_model_1548765213" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,8 @@
     <sheet name="trained_model_1548841707" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="trained_model_1548842498" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="trained_model_1548999475" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="trained_model_1548999930" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="trained_model_1549000271" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="8">
   <si>
     <t xml:space="preserve">Hasil analisis</t>
   </si>
@@ -47,6 +49,9 @@
   <si>
     <t xml:space="preserve">The accuracy is: 0.3333333333333333</t>
   </si>
+  <si>
+    <t xml:space="preserve">accuracy</t>
+  </si>
 </sst>
 </file>
 
@@ -55,7 +60,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -79,6 +84,11 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -212,7 +222,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -222,214 +232,13 @@
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>trained_model_1548765213!$B$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>pos</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>trained_model_1548765213!$A$4:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>pos</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>neg</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>neu</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>trained_model_1548765213!$B$4:$B$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>trained_model_1548765213!$C$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>neg</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff420e"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>trained_model_1548765213!$A$4:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>pos</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>neg</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>neu</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>trained_model_1548765213!$C$4:$C$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>trained_model_1548765213!$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>neu</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ffd320"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>trained_model_1548765213!$A$4:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>pos</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>neg</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>neu</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>trained_model_1548765213!$D$4:$D$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="73611311"/>
-        <c:axId val="92904779"/>
+        <c:axId val="5580658"/>
+        <c:axId val="81446725"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="73611311"/>
+        <c:axId val="5580658"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -464,14 +273,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92904779"/>
+        <c:crossAx val="81446725"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92904779"/>
+        <c:axId val="81446725"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -515,7 +324,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73611311"/>
+        <c:crossAx val="5580658"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -552,7 +361,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -567,11 +376,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>trained_model_1548767100!$B$3</c:f>
+              <c:f>trained_model_1548841707!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>pos</c:v>
+                  <c:v>neg</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -595,9 +404,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>trained_model_1548767100!$A$4:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
+              <c:f>trained_model_1548841707!$A$3:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>pos</c:v>
                 </c:pt>
@@ -606,24 +415,33 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>neu</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>trained_model_1548767100!$B$4:$B$6</c:f>
+              <c:f>trained_model_1548841707!$C$3:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -634,11 +452,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>trained_model_1548767100!$C$3</c:f>
+              <c:f>trained_model_1548841707!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>neg</c:v>
+                  <c:v>neu</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -662,9 +480,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>trained_model_1548767100!$A$4:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
+              <c:f>trained_model_1548841707!$A$3:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>pos</c:v>
                 </c:pt>
@@ -673,91 +491,33 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>neu</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>trained_model_1548767100!$C$4:$C$6</c:f>
+              <c:f>trained_model_1548841707!$D$3:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>trained_model_1548767100!$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>neu</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ffd320"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>trained_model_1548767100!$A$4:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>pos</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>neg</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>neu</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>trained_model_1548767100!$D$4:$D$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -765,11 +525,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="34676956"/>
-        <c:axId val="3830963"/>
+        <c:axId val="85637576"/>
+        <c:axId val="80146620"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="34676956"/>
+        <c:axId val="85637576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -804,14 +564,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3830963"/>
+        <c:crossAx val="80146620"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3830963"/>
+        <c:axId val="80146620"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,7 +615,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34676956"/>
+        <c:crossAx val="85637576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -892,7 +652,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -907,11 +667,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>trained_model_1548835538!$B$2</c:f>
+              <c:f>trained_model_1548842498!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>pos</c:v>
+                  <c:v>neg</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -935,9 +695,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>trained_model_1548835538!$A$3:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
+              <c:f>trained_model_1548842498!$A$3:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>pos</c:v>
                 </c:pt>
@@ -946,24 +706,33 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>neu</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>trained_model_1548835538!$B$3:$B$5</c:f>
+              <c:f>trained_model_1548842498!$C$3:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -974,11 +743,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>trained_model_1548835538!$C$2</c:f>
+              <c:f>trained_model_1548842498!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>neg</c:v>
+                  <c:v>neu</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1002,9 +771,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>trained_model_1548835538!$A$3:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
+              <c:f>trained_model_1548842498!$A$3:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>pos</c:v>
                 </c:pt>
@@ -1013,91 +782,33 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>neu</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>trained_model_1548835538!$C$3:$C$5</c:f>
+              <c:f>trained_model_1548842498!$D$3:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>trained_model_1548835538!$D$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>neu</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ffd320"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>trained_model_1548835538!$A$3:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>pos</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>neg</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>neu</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>trained_model_1548835538!$D$3:$D$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1105,11 +816,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="92470126"/>
-        <c:axId val="45196696"/>
+        <c:axId val="17869123"/>
+        <c:axId val="31472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92470126"/>
+        <c:axId val="17869123"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1144,14 +855,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45196696"/>
+        <c:crossAx val="31472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45196696"/>
+        <c:axId val="31472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1195,7 +906,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92470126"/>
+        <c:crossAx val="17869123"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1232,7 +943,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1242,13 +953,214 @@
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>trained_model_1548999930!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>trained_model_1548999930!$A$4:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>pos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>neg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>neu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>trained_model_1548999930!$B$4:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>trained_model_1548999930!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>neg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>trained_model_1548999930!$A$4:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>pos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>neg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>neu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>trained_model_1548999930!$C$4:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>trained_model_1548999930!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>neu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>trained_model_1548999930!$A$4:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>pos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>neg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>neu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>trained_model_1548999930!$D$4:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="2236258"/>
-        <c:axId val="43049261"/>
+        <c:axId val="65577"/>
+        <c:axId val="12405550"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2236258"/>
+        <c:axId val="65577"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1283,14 +1195,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43049261"/>
+        <c:crossAx val="12405550"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43049261"/>
+        <c:axId val="12405550"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1334,7 +1246,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2236258"/>
+        <c:crossAx val="65577"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1371,11 +1283,50 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>PEMETAAN HASIL PREDIKSI</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:barChart>
         <c:barDir val="col"/>
@@ -1386,11 +1337,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>trained_model_1548841707!$C$2</c:f>
+              <c:f>trained_model_1549000271!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>neg</c:v>
+                  <c:v>pos</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1414,9 +1365,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>trained_model_1548841707!$A$3:$B$5</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+              <c:f>trained_model_1549000271!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>pos</c:v>
                 </c:pt>
@@ -1425,33 +1376,24 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>neu</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>trained_model_1548841707!$C$3:$C$5</c:f>
+              <c:f>trained_model_1549000271!$B$3:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1462,11 +1404,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>trained_model_1548841707!$D$2</c:f>
+              <c:f>trained_model_1549000271!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>neu</c:v>
+                  <c:v>neg</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1490,9 +1432,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>trained_model_1548841707!$A$3:$B$5</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+              <c:f>trained_model_1549000271!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>pos</c:v>
                 </c:pt>
@@ -1501,33 +1443,91 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>neu</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>trained_model_1548841707!$D$3:$D$5</c:f>
+              <c:f>trained_model_1549000271!$C$3:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>trained_model_1549000271!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>neu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>trained_model_1549000271!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>pos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>neg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>neu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>trained_model_1549000271!$D$3:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1535,11 +1535,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="61559887"/>
-        <c:axId val="51425697"/>
+        <c:axId val="28828738"/>
+        <c:axId val="2238171"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61559887"/>
+        <c:axId val="28828738"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1574,14 +1574,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51425697"/>
+        <c:crossAx val="2238171"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51425697"/>
+        <c:axId val="2238171"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1625,7 +1625,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61559887"/>
+        <c:crossAx val="28828738"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1662,7 +1662,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1677,11 +1677,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>trained_model_1548842498!$C$2</c:f>
+              <c:f>trained_model_1548765213!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>neg</c:v>
+                  <c:v>pos</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1705,9 +1705,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>trained_model_1548842498!$A$3:$B$5</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+              <c:f>trained_model_1548765213!$A$4:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>pos</c:v>
                 </c:pt>
@@ -1716,33 +1716,24 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>neu</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>trained_model_1548842498!$C$3:$C$5</c:f>
+              <c:f>trained_model_1548765213!$B$4:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1753,11 +1744,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>trained_model_1548842498!$D$2</c:f>
+              <c:f>trained_model_1548765213!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>neu</c:v>
+                  <c:v>neg</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1781,9 +1772,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>trained_model_1548842498!$A$3:$B$5</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+              <c:f>trained_model_1548765213!$A$4:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>pos</c:v>
                 </c:pt>
@@ -1792,33 +1783,91 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>neu</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>trained_model_1548842498!$D$3:$D$5</c:f>
+              <c:f>trained_model_1548765213!$C$4:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>trained_model_1548765213!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>neu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>trained_model_1548765213!$A$4:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>pos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>neg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>neu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>trained_model_1548765213!$D$4:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1826,11 +1875,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="70299878"/>
-        <c:axId val="68242017"/>
+        <c:axId val="17339301"/>
+        <c:axId val="39296097"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70299878"/>
+        <c:axId val="17339301"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1865,14 +1914,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68242017"/>
+        <c:crossAx val="39296097"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68242017"/>
+        <c:axId val="39296097"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1916,7 +1965,726 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70299878"/>
+        <c:crossAx val="17339301"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>trained_model_1548767100!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>trained_model_1548767100!$A$4:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>pos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>neg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>neu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>trained_model_1548767100!$B$4:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>trained_model_1548767100!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>neg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>trained_model_1548767100!$A$4:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>pos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>neg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>neu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>trained_model_1548767100!$C$4:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>trained_model_1548767100!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>neu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>trained_model_1548767100!$A$4:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>pos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>neg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>neu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>trained_model_1548767100!$D$4:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="53430098"/>
+        <c:axId val="71230922"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="53430098"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="71230922"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="71230922"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="53430098"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>PEMETAAN HASIL PREDIKSI</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>trained_model_1548835538!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>trained_model_1548835538!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>pos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>neg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>neu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>trained_model_1548835538!$B$3:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>trained_model_1548835538!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>neg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>trained_model_1548835538!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>pos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>neg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>neu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>trained_model_1548835538!$C$3:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>trained_model_1548835538!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>neu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>trained_model_1548835538!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>pos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>neg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>neu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>trained_model_1548835538!$D$3:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="44316592"/>
+        <c:axId val="76846729"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="44316592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="76846729"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="76846729"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="44316592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2158,6 +2926,76 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>36360</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>36000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>106560</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>24480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="3287520" y="361080"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>46800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>74160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>116640</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>62640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="4110480" y="886680"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -2308,10 +3146,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:D5"/>
+  <dimension ref="A2:D8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N9" activeCellId="0" sqref="N9"/>
+      <selection pane="topLeft" activeCell="N21" activeCellId="0" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2370,6 +3208,26 @@
       </c>
       <c r="D5" s="1" t="n">
         <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <f aca="false">SUM(B3:B5)</f>
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <f aca="false">SUM(C3:C5)</f>
+        <v>26</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">SUM(D3:D5)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="n">
+        <f aca="false">SUM(B6:D6)</f>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2543,7 +3401,7 @@
   </sheetPr>
   <dimension ref="A2:D7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -2607,4 +3465,176 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A3:D9"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.38</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:D7"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N22" activeCellId="0" sqref="N22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>